<commit_message>
Flags and callbacks names
</commit_message>
<xml_diff>
--- a/src/test/resources/MyFirstExcel.xlsx
+++ b/src/test/resources/MyFirstExcel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t xml:space="preserve">Case Ref</t>
   </si>
@@ -34,7 +34,10 @@
     <t xml:space="preserve">Flag2</t>
   </si>
   <si>
-    <t xml:space="preserve">EQP</t>
+    <t xml:space="preserve">Flag3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag4</t>
   </si>
   <si>
     <t xml:space="preserve">1820000/2019</t>
@@ -76,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -135,16 +139,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -165,20 +165,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -194,82 +194,91 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" error="Cannot change the value" errorTitle="Not Applicable" operator="between" showDropDown="true" showErrorMessage="true" showInputMessage="false" sqref="A1:IQ1 A2:A1007" type="list">
+    <dataValidation allowBlank="true" error="Cannot change the value" errorTitle="Not Applicable" operator="between" showDropDown="true" showErrorMessage="true" showInputMessage="false" sqref="A1:D1 G1:IQ1 A2:A8 D2:F2 E3:F7 A9:A1007" type="list">
       <formula1>"qwer%yuiop_1234567890"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>